<commit_message>
Criação de tela Evidências ML
</commit_message>
<xml_diff>
--- a/database/seeders/StdSeeders/orc_treinados.xlsx
+++ b/database/seeders/StdSeeders/orc_treinados.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjetoTelaML\proj-tela-ml\database\seeders\StdSeeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B806D68-54F8-43C6-8AED-BCC4C127F5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC98F85C-DCF5-4D50-9E29-89F68FB7BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19935" yWindow="2100" windowWidth="15375" windowHeight="7965" xr2:uid="{E622950E-4AAC-41EE-A53A-3F64FFA2B5C0}"/>
+    <workbookView xWindow="-28920" yWindow="-4815" windowWidth="29040" windowHeight="15840" xr2:uid="{E622950E-4AAC-41EE-A53A-3F64FFA2B5C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$C$173</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$C$172</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="233">
   <si>
     <t>numero_orcamento</t>
   </si>
@@ -672,6 +672,72 @@
   </si>
   <si>
     <t>0001</t>
+  </si>
+  <si>
+    <t>3079F</t>
+  </si>
+  <si>
+    <t>2631E</t>
+  </si>
+  <si>
+    <t>8448</t>
+  </si>
+  <si>
+    <t>3073F</t>
+  </si>
+  <si>
+    <t>8521</t>
+  </si>
+  <si>
+    <t>2641E</t>
+  </si>
+  <si>
+    <t>8506</t>
+  </si>
+  <si>
+    <t>8527</t>
+  </si>
+  <si>
+    <t>8536</t>
+  </si>
+  <si>
+    <t>8537</t>
+  </si>
+  <si>
+    <t>3111F</t>
+  </si>
+  <si>
+    <t>3118F</t>
+  </si>
+  <si>
+    <t>3116F</t>
+  </si>
+  <si>
+    <t>2680E</t>
+  </si>
+  <si>
+    <t>8554</t>
+  </si>
+  <si>
+    <t>3131F</t>
+  </si>
+  <si>
+    <t>8569</t>
+  </si>
+  <si>
+    <t>8573</t>
+  </si>
+  <si>
+    <t>2715E</t>
+  </si>
+  <si>
+    <t>3140F</t>
+  </si>
+  <si>
+    <t>3139F</t>
+  </si>
+  <si>
+    <t>8576</t>
   </si>
 </sst>
 </file>
@@ -1044,15 +1110,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7EBF668-6535-4FB5-869E-A735B13FF3CF}">
-  <dimension ref="A1:C328"/>
+  <dimension ref="A1:C359"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
-      <selection activeCell="G327" sqref="G327"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G349" sqref="G349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2530,8 +2597,8 @@
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135">
-        <v>9999</v>
+      <c r="A135" t="s">
+        <v>136</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -2542,7 +2609,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -2553,7 +2620,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -2563,8 +2630,8 @@
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>138</v>
+      <c r="A138">
+        <v>8475</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -2575,7 +2642,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>8475</v>
+        <v>8489</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -2586,7 +2653,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>8489</v>
+        <v>8506</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -2597,7 +2664,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>8506</v>
+        <v>7271</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -2608,7 +2675,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>7271</v>
+        <v>7722</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -2619,7 +2686,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>7722</v>
+        <v>7986</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -2630,7 +2697,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>7986</v>
+        <v>8050</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -2641,7 +2708,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>8050</v>
+        <v>8137</v>
       </c>
       <c r="B145">
         <v>0</v>
@@ -2652,7 +2719,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>8137</v>
+        <v>8180</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -2663,7 +2730,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>8180</v>
+        <v>8191</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -2674,7 +2741,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>8191</v>
+        <v>8194</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -2685,7 +2752,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>8194</v>
+        <v>8223</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -2696,7 +2763,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>8223</v>
+        <v>5659</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -2707,7 +2774,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>5659</v>
+        <v>6158</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -2718,7 +2785,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>6158</v>
+        <v>7464</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -2729,7 +2796,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>7464</v>
+        <v>7526</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -2740,7 +2807,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>7526</v>
+        <v>7640</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -2751,7 +2818,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>7640</v>
+        <v>7894</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -2762,7 +2829,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>7894</v>
+        <v>7969</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -2773,7 +2840,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>7969</v>
+        <v>8031</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -2784,7 +2851,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>8031</v>
+        <v>8094</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -2795,7 +2862,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>8094</v>
+        <v>8174</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -2806,7 +2873,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>8174</v>
+        <v>8185</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -2817,7 +2884,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>8185</v>
+        <v>8311</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -2827,8 +2894,8 @@
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162">
-        <v>8311</v>
+      <c r="A162" t="s">
+        <v>139</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -2838,8 +2905,8 @@
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>139</v>
+      <c r="A163">
+        <v>7937</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -2850,7 +2917,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>7937</v>
+        <v>7917</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -2860,8 +2927,8 @@
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165">
-        <v>7917</v>
+      <c r="A165" t="s">
+        <v>140</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -2871,8 +2938,8 @@
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>140</v>
+      <c r="A166">
+        <v>8416</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -2883,7 +2950,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>8416</v>
+        <v>8491</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -2893,8 +2960,8 @@
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168">
-        <v>8491</v>
+      <c r="A168" t="s">
+        <v>141</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -2904,8 +2971,8 @@
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>141</v>
+      <c r="A169">
+        <v>7702</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -2916,7 +2983,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>7702</v>
+        <v>8114</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -2927,7 +2994,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>8114</v>
+        <v>5641</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -2938,7 +3005,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>5641</v>
+        <v>7257</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -2949,7 +3016,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>7257</v>
+        <v>7471</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -2960,7 +3027,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>7471</v>
+        <v>7873</v>
       </c>
       <c r="B174">
         <v>0</v>
@@ -2971,7 +3038,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>7873</v>
+        <v>7962</v>
       </c>
       <c r="B175">
         <v>0</v>
@@ -2982,7 +3049,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>7962</v>
+        <v>7967</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -2993,7 +3060,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>7967</v>
+        <v>8049</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -3004,7 +3071,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>8049</v>
+        <v>8055</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -3015,7 +3082,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>8055</v>
+        <v>8068</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -3026,7 +3093,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>8068</v>
+        <v>8076</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -3037,7 +3104,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>8076</v>
+        <v>8121</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -3048,7 +3115,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>8121</v>
+        <v>8133</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -3059,7 +3126,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>8133</v>
+        <v>8146</v>
       </c>
       <c r="B183">
         <v>0</v>
@@ -3070,7 +3137,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>8146</v>
+        <v>8148</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -3081,7 +3148,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>8148</v>
+        <v>8160</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -3092,7 +3159,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>8160</v>
+        <v>8256</v>
       </c>
       <c r="B186">
         <v>0</v>
@@ -3103,7 +3170,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>8256</v>
+        <v>8268</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -3114,7 +3181,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>8268</v>
+        <v>8305</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -3125,7 +3192,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>8305</v>
+        <v>8333</v>
       </c>
       <c r="B189">
         <v>0</v>
@@ -3136,7 +3203,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190">
-        <v>8333</v>
+        <v>7887</v>
       </c>
       <c r="B190">
         <v>0</v>
@@ -3147,7 +3214,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>7887</v>
+        <v>6342</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -3158,7 +3225,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>6342</v>
+        <v>7717</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -3168,8 +3235,8 @@
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193">
-        <v>7717</v>
+      <c r="A193" t="s">
+        <v>142</v>
       </c>
       <c r="B193">
         <v>0</v>
@@ -3180,7 +3247,7 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B194">
         <v>0</v>
@@ -3191,7 +3258,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B195">
         <v>0</v>
@@ -3202,7 +3269,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B196">
         <v>0</v>
@@ -3213,7 +3280,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B197">
         <v>0</v>
@@ -3224,7 +3291,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B198">
         <v>0</v>
@@ -3235,7 +3302,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B199">
         <v>0</v>
@@ -3246,7 +3313,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B200">
         <v>0</v>
@@ -3257,7 +3324,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B201">
         <v>0</v>
@@ -3268,7 +3335,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B202">
         <v>0</v>
@@ -3279,7 +3346,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B203">
         <v>0</v>
@@ -3290,7 +3357,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B204">
         <v>0</v>
@@ -3301,7 +3368,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B205">
         <v>0</v>
@@ -3312,7 +3379,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B206">
         <v>0</v>
@@ -3323,7 +3390,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B207">
         <v>0</v>
@@ -3334,7 +3401,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B208">
         <v>0</v>
@@ -3345,7 +3412,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B209">
         <v>0</v>
@@ -3356,7 +3423,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B210">
         <v>0</v>
@@ -3367,7 +3434,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B211">
         <v>0</v>
@@ -3378,7 +3445,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B212">
         <v>0</v>
@@ -3389,7 +3456,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B213">
         <v>0</v>
@@ -3400,7 +3467,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B214">
         <v>0</v>
@@ -3411,7 +3478,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B215">
         <v>0</v>
@@ -3422,7 +3489,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B216">
         <v>0</v>
@@ -3433,7 +3500,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B217">
         <v>0</v>
@@ -3444,7 +3511,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B218">
         <v>0</v>
@@ -3455,7 +3522,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B219">
         <v>0</v>
@@ -3466,7 +3533,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B220">
         <v>0</v>
@@ -3477,7 +3544,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B221">
         <v>0</v>
@@ -3488,7 +3555,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B222">
         <v>0</v>
@@ -3499,7 +3566,7 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B223">
         <v>0</v>
@@ -3510,7 +3577,7 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B224">
         <v>0</v>
@@ -3521,7 +3588,7 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B225">
         <v>0</v>
@@ -3532,7 +3599,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B226">
         <v>0</v>
@@ -3543,7 +3610,7 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B227">
         <v>0</v>
@@ -3554,7 +3621,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B228">
         <v>0</v>
@@ -3565,7 +3632,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B229">
         <v>0</v>
@@ -3576,7 +3643,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B230">
         <v>0</v>
@@ -3587,7 +3654,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B231">
         <v>0</v>
@@ -3598,7 +3665,7 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B232">
         <v>0</v>
@@ -3609,7 +3676,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B233">
         <v>0</v>
@@ -3620,7 +3687,7 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B234">
         <v>0</v>
@@ -3631,7 +3698,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B235">
         <v>0</v>
@@ -3642,7 +3709,7 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B236">
         <v>0</v>
@@ -3653,7 +3720,7 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B237">
         <v>0</v>
@@ -3663,8 +3730,8 @@
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>186</v>
+      <c r="A238">
+        <v>7911</v>
       </c>
       <c r="B238">
         <v>0</v>
@@ -3675,7 +3742,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239">
-        <v>7911</v>
+        <v>8140</v>
       </c>
       <c r="B239">
         <v>0</v>
@@ -3685,8 +3752,8 @@
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A240">
-        <v>8140</v>
+      <c r="A240" t="s">
+        <v>187</v>
       </c>
       <c r="B240">
         <v>0</v>
@@ -3697,7 +3764,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B241">
         <v>0</v>
@@ -3708,7 +3775,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B242">
         <v>0</v>
@@ -3719,7 +3786,7 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B243">
         <v>0</v>
@@ -3729,8 +3796,8 @@
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
-        <v>190</v>
+      <c r="A244">
+        <v>6722</v>
       </c>
       <c r="B244">
         <v>0</v>
@@ -3741,7 +3808,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245">
-        <v>6722</v>
+        <v>7056</v>
       </c>
       <c r="B245">
         <v>0</v>
@@ -3752,7 +3819,7 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246">
-        <v>7056</v>
+        <v>7202</v>
       </c>
       <c r="B246">
         <v>0</v>
@@ -3763,7 +3830,7 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247">
-        <v>7202</v>
+        <v>6903</v>
       </c>
       <c r="B247">
         <v>0</v>
@@ -3773,8 +3840,8 @@
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A248">
-        <v>6903</v>
+      <c r="A248" t="s">
+        <v>191</v>
       </c>
       <c r="B248">
         <v>0</v>
@@ -3784,8 +3851,8 @@
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>191</v>
+      <c r="A249">
+        <v>7248</v>
       </c>
       <c r="B249">
         <v>0</v>
@@ -3795,8 +3862,8 @@
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A250">
-        <v>7248</v>
+      <c r="A250" t="s">
+        <v>192</v>
       </c>
       <c r="B250">
         <v>0</v>
@@ -3806,8 +3873,8 @@
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
-        <v>192</v>
+      <c r="A251">
+        <v>5525</v>
       </c>
       <c r="B251">
         <v>0</v>
@@ -3818,7 +3885,7 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252">
-        <v>5525</v>
+        <v>5513</v>
       </c>
       <c r="B252">
         <v>0</v>
@@ -3828,8 +3895,8 @@
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A253">
-        <v>5513</v>
+      <c r="A253" t="s">
+        <v>193</v>
       </c>
       <c r="B253">
         <v>0</v>
@@ -3840,7 +3907,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B254">
         <v>0</v>
@@ -3851,7 +3918,7 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B255">
         <v>0</v>
@@ -3862,7 +3929,7 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B256">
         <v>0</v>
@@ -3872,8 +3939,8 @@
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
-        <v>196</v>
+      <c r="A257">
+        <v>7031</v>
       </c>
       <c r="B257">
         <v>0</v>
@@ -3884,7 +3951,7 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258">
-        <v>7031</v>
+        <v>7065</v>
       </c>
       <c r="B258">
         <v>0</v>
@@ -3895,7 +3962,7 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259">
-        <v>7065</v>
+        <v>7097</v>
       </c>
       <c r="B259">
         <v>0</v>
@@ -3906,7 +3973,7 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260">
-        <v>7097</v>
+        <v>7177</v>
       </c>
       <c r="B260">
         <v>0</v>
@@ -3917,7 +3984,7 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261">
-        <v>7177</v>
+        <v>7226</v>
       </c>
       <c r="B261">
         <v>0</v>
@@ -3928,7 +3995,7 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262">
-        <v>7226</v>
+        <v>7230</v>
       </c>
       <c r="B262">
         <v>0</v>
@@ -3938,8 +4005,8 @@
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A263">
-        <v>7230</v>
+      <c r="A263" t="s">
+        <v>197</v>
       </c>
       <c r="B263">
         <v>0</v>
@@ -3949,8 +4016,8 @@
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A264" t="s">
-        <v>197</v>
+      <c r="A264">
+        <v>7332</v>
       </c>
       <c r="B264">
         <v>0</v>
@@ -3961,7 +4028,7 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265">
-        <v>7332</v>
+        <v>7334</v>
       </c>
       <c r="B265">
         <v>0</v>
@@ -3972,7 +4039,7 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266">
-        <v>7334</v>
+        <v>7346</v>
       </c>
       <c r="B266">
         <v>0</v>
@@ -3983,7 +4050,7 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267">
-        <v>7346</v>
+        <v>7385</v>
       </c>
       <c r="B267">
         <v>0</v>
@@ -3994,7 +4061,7 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268">
-        <v>7385</v>
+        <v>7457</v>
       </c>
       <c r="B268">
         <v>0</v>
@@ -4005,7 +4072,7 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269">
-        <v>7457</v>
+        <v>7466</v>
       </c>
       <c r="B269">
         <v>0</v>
@@ -4015,8 +4082,8 @@
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A270">
-        <v>7466</v>
+      <c r="A270" t="s">
+        <v>198</v>
       </c>
       <c r="B270">
         <v>0</v>
@@ -4027,7 +4094,7 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B271">
         <v>0</v>
@@ -4038,7 +4105,7 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B272">
         <v>0</v>
@@ -4048,8 +4115,8 @@
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A273" t="s">
-        <v>200</v>
+      <c r="A273">
+        <v>7598</v>
       </c>
       <c r="B273">
         <v>0</v>
@@ -4060,7 +4127,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274">
-        <v>7598</v>
+        <v>7606</v>
       </c>
       <c r="B274">
         <v>0</v>
@@ -4071,7 +4138,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275">
-        <v>7606</v>
+        <v>7610</v>
       </c>
       <c r="B275">
         <v>0</v>
@@ -4082,7 +4149,7 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276">
-        <v>7610</v>
+        <v>7627</v>
       </c>
       <c r="B276">
         <v>0</v>
@@ -4093,7 +4160,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277">
-        <v>7627</v>
+        <v>7634</v>
       </c>
       <c r="B277">
         <v>0</v>
@@ -4104,7 +4171,7 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278">
-        <v>7634</v>
+        <v>7636</v>
       </c>
       <c r="B278">
         <v>0</v>
@@ -4114,8 +4181,8 @@
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A279">
-        <v>7636</v>
+      <c r="A279" t="s">
+        <v>201</v>
       </c>
       <c r="B279">
         <v>0</v>
@@ -4125,8 +4192,8 @@
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
-        <v>201</v>
+      <c r="A280">
+        <v>7677</v>
       </c>
       <c r="B280">
         <v>0</v>
@@ -4136,8 +4203,8 @@
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A281">
-        <v>7677</v>
+      <c r="A281" t="s">
+        <v>202</v>
       </c>
       <c r="B281">
         <v>0</v>
@@ -4147,8 +4214,8 @@
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A282" t="s">
-        <v>202</v>
+      <c r="A282">
+        <v>7746</v>
       </c>
       <c r="B282">
         <v>0</v>
@@ -4159,7 +4226,7 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283">
-        <v>7746</v>
+        <v>7792</v>
       </c>
       <c r="B283">
         <v>0</v>
@@ -4170,7 +4237,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284">
-        <v>7792</v>
+        <v>7885</v>
       </c>
       <c r="B284">
         <v>0</v>
@@ -4181,7 +4248,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285">
-        <v>7885</v>
+        <v>7888</v>
       </c>
       <c r="B285">
         <v>0</v>
@@ -4192,7 +4259,7 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286">
-        <v>7888</v>
+        <v>7913</v>
       </c>
       <c r="B286">
         <v>0</v>
@@ -4203,7 +4270,7 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287">
-        <v>7913</v>
+        <v>7963</v>
       </c>
       <c r="B287">
         <v>0</v>
@@ -4214,7 +4281,7 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288">
-        <v>7963</v>
+        <v>7966</v>
       </c>
       <c r="B288">
         <v>0</v>
@@ -4225,7 +4292,7 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289">
-        <v>7966</v>
+        <v>7979</v>
       </c>
       <c r="B289">
         <v>0</v>
@@ -4235,8 +4302,8 @@
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A290">
-        <v>7979</v>
+      <c r="A290" t="s">
+        <v>203</v>
       </c>
       <c r="B290">
         <v>0</v>
@@ -4247,7 +4314,7 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B291">
         <v>0</v>
@@ -4258,7 +4325,7 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B292">
         <v>0</v>
@@ -4269,7 +4336,7 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B293">
         <v>0</v>
@@ -4279,8 +4346,8 @@
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
-        <v>206</v>
+      <c r="A294">
+        <v>5502</v>
       </c>
       <c r="B294">
         <v>0</v>
@@ -4291,7 +4358,7 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295">
-        <v>5502</v>
+        <v>5514</v>
       </c>
       <c r="B295">
         <v>0</v>
@@ -4302,7 +4369,7 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296">
-        <v>5514</v>
+        <v>5522</v>
       </c>
       <c r="B296">
         <v>0</v>
@@ -4312,8 +4379,8 @@
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A297">
-        <v>5522</v>
+      <c r="A297" t="s">
+        <v>207</v>
       </c>
       <c r="B297">
         <v>0</v>
@@ -4323,8 +4390,8 @@
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
-        <v>207</v>
+      <c r="A298">
+        <v>5547</v>
       </c>
       <c r="B298">
         <v>0</v>
@@ -4335,7 +4402,7 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299">
-        <v>5547</v>
+        <v>5550</v>
       </c>
       <c r="B299">
         <v>0</v>
@@ -4346,7 +4413,7 @@
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300">
-        <v>5550</v>
+        <v>5657</v>
       </c>
       <c r="B300">
         <v>0</v>
@@ -4357,7 +4424,7 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301">
-        <v>5657</v>
+        <v>5723</v>
       </c>
       <c r="B301">
         <v>0</v>
@@ -4368,7 +4435,7 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302">
-        <v>5723</v>
+        <v>6065</v>
       </c>
       <c r="B302">
         <v>0</v>
@@ -4379,7 +4446,7 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303">
-        <v>6065</v>
+        <v>6129</v>
       </c>
       <c r="B303">
         <v>0</v>
@@ -4389,8 +4456,8 @@
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A304">
-        <v>6129</v>
+      <c r="A304" t="s">
+        <v>208</v>
       </c>
       <c r="B304">
         <v>0</v>
@@ -4400,8 +4467,8 @@
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A305" t="s">
-        <v>208</v>
+      <c r="A305">
+        <v>6135</v>
       </c>
       <c r="B305">
         <v>0</v>
@@ -4412,7 +4479,7 @@
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306">
-        <v>6135</v>
+        <v>6167</v>
       </c>
       <c r="B306">
         <v>0</v>
@@ -4423,7 +4490,7 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307">
-        <v>6167</v>
+        <v>6177</v>
       </c>
       <c r="B307">
         <v>0</v>
@@ -4434,7 +4501,7 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308">
-        <v>6177</v>
+        <v>6216</v>
       </c>
       <c r="B308">
         <v>0</v>
@@ -4445,7 +4512,7 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309">
-        <v>6216</v>
+        <v>6539</v>
       </c>
       <c r="B309">
         <v>0</v>
@@ -4456,7 +4523,7 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310">
-        <v>6539</v>
+        <v>6623</v>
       </c>
       <c r="B310">
         <v>0</v>
@@ -4467,7 +4534,7 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311">
-        <v>6623</v>
+        <v>6627</v>
       </c>
       <c r="B311">
         <v>0</v>
@@ -4478,7 +4545,7 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312">
-        <v>6627</v>
+        <v>6899</v>
       </c>
       <c r="B312">
         <v>0</v>
@@ -4489,7 +4556,7 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313">
-        <v>6899</v>
+        <v>6990</v>
       </c>
       <c r="B313">
         <v>0</v>
@@ -4500,7 +4567,7 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314">
-        <v>6990</v>
+        <v>7057</v>
       </c>
       <c r="B314">
         <v>0</v>
@@ -4511,7 +4578,7 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315">
-        <v>7057</v>
+        <v>7113</v>
       </c>
       <c r="B315">
         <v>0</v>
@@ -4522,7 +4589,7 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316">
-        <v>7113</v>
+        <v>7243</v>
       </c>
       <c r="B316">
         <v>0</v>
@@ -4533,7 +4600,7 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317">
-        <v>7243</v>
+        <v>7444</v>
       </c>
       <c r="B317">
         <v>0</v>
@@ -4544,7 +4611,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318">
-        <v>7444</v>
+        <v>6866</v>
       </c>
       <c r="B318">
         <v>0</v>
@@ -4555,7 +4622,7 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319">
-        <v>6866</v>
+        <v>7063</v>
       </c>
       <c r="B319">
         <v>0</v>
@@ -4566,7 +4633,7 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320">
-        <v>7063</v>
+        <v>6131</v>
       </c>
       <c r="B320">
         <v>0</v>
@@ -4577,7 +4644,7 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321">
-        <v>6131</v>
+        <v>8385</v>
       </c>
       <c r="B321">
         <v>0</v>
@@ -4588,7 +4655,7 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322">
-        <v>8385</v>
+        <v>8189</v>
       </c>
       <c r="B322">
         <v>0</v>
@@ -4599,7 +4666,7 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323">
-        <v>8189</v>
+        <v>2338</v>
       </c>
       <c r="B323">
         <v>0</v>
@@ -4609,8 +4676,8 @@
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A324">
-        <v>2338</v>
+      <c r="A324" t="s">
+        <v>209</v>
       </c>
       <c r="B324">
         <v>0</v>
@@ -4620,8 +4687,8 @@
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A325" t="s">
-        <v>209</v>
+      <c r="A325">
+        <v>7241</v>
       </c>
       <c r="B325">
         <v>0</v>
@@ -4632,7 +4699,7 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326">
-        <v>7241</v>
+        <v>8537</v>
       </c>
       <c r="B326">
         <v>0</v>
@@ -4642,29 +4709,370 @@
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A327">
-        <v>8537</v>
+      <c r="A327" t="s">
+        <v>211</v>
       </c>
       <c r="B327">
         <v>0</v>
       </c>
       <c r="C327">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A328" s="1" t="s">
+      <c r="A328" t="s">
+        <v>212</v>
+      </c>
+      <c r="B328">
+        <v>0</v>
+      </c>
+      <c r="C328">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>213</v>
+      </c>
+      <c r="B329">
+        <v>0</v>
+      </c>
+      <c r="C329">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>214</v>
+      </c>
+      <c r="B330">
+        <v>0</v>
+      </c>
+      <c r="C330">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>215</v>
+      </c>
+      <c r="B331">
+        <v>0</v>
+      </c>
+      <c r="C331">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>216</v>
+      </c>
+      <c r="B332">
+        <v>0</v>
+      </c>
+      <c r="C332">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>217</v>
+      </c>
+      <c r="B333">
+        <v>0</v>
+      </c>
+      <c r="C333">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>217</v>
+      </c>
+      <c r="B334">
+        <v>1</v>
+      </c>
+      <c r="C334">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>217</v>
+      </c>
+      <c r="B335">
+        <v>2</v>
+      </c>
+      <c r="C335">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>218</v>
+      </c>
+      <c r="B336">
+        <v>0</v>
+      </c>
+      <c r="C336">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>218</v>
+      </c>
+      <c r="B337">
+        <v>1</v>
+      </c>
+      <c r="C337">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>217</v>
+      </c>
+      <c r="B338">
+        <v>3</v>
+      </c>
+      <c r="C338">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>219</v>
+      </c>
+      <c r="B339">
+        <v>0</v>
+      </c>
+      <c r="C339">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>220</v>
+      </c>
+      <c r="B340">
+        <v>0</v>
+      </c>
+      <c r="C340">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>219</v>
+      </c>
+      <c r="B341">
+        <v>1</v>
+      </c>
+      <c r="C341">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>218</v>
+      </c>
+      <c r="B342">
+        <v>2</v>
+      </c>
+      <c r="C342">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>221</v>
+      </c>
+      <c r="B343">
+        <v>0</v>
+      </c>
+      <c r="C343">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>222</v>
+      </c>
+      <c r="B344">
+        <v>0</v>
+      </c>
+      <c r="C344">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>220</v>
+      </c>
+      <c r="B345">
+        <v>1</v>
+      </c>
+      <c r="C345">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>223</v>
+      </c>
+      <c r="B346">
+        <v>0</v>
+      </c>
+      <c r="C346">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>224</v>
+      </c>
+      <c r="B347">
+        <v>0</v>
+      </c>
+      <c r="C347">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>8542</v>
+      </c>
+      <c r="B348">
+        <v>0</v>
+      </c>
+      <c r="C348">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>225</v>
+      </c>
+      <c r="B349">
+        <v>0</v>
+      </c>
+      <c r="C349">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>226</v>
+      </c>
+      <c r="B350">
+        <v>0</v>
+      </c>
+      <c r="C350">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>225</v>
+      </c>
+      <c r="B351">
+        <v>1</v>
+      </c>
+      <c r="C351">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>225</v>
+      </c>
+      <c r="B352">
+        <v>2</v>
+      </c>
+      <c r="C352">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>227</v>
+      </c>
+      <c r="B353">
+        <v>0</v>
+      </c>
+      <c r="C353">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>228</v>
+      </c>
+      <c r="B354">
+        <v>0</v>
+      </c>
+      <c r="C354">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>229</v>
+      </c>
+      <c r="B355">
+        <v>0</v>
+      </c>
+      <c r="C355">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>230</v>
+      </c>
+      <c r="B356">
+        <v>0</v>
+      </c>
+      <c r="C356">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>231</v>
+      </c>
+      <c r="B357">
+        <v>0</v>
+      </c>
+      <c r="C357">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>232</v>
+      </c>
+      <c r="B358">
+        <v>0</v>
+      </c>
+      <c r="C358">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A359" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B328">
-        <v>0</v>
-      </c>
-      <c r="C328">
+      <c r="B359">
+        <v>0</v>
+      </c>
+      <c r="C359">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C173" xr:uid="{F7EBF668-6535-4FB5-869E-A735B13FF3CF}"/>
+  <autoFilter ref="A1:C172" xr:uid="{F7EBF668-6535-4FB5-869E-A735B13FF3CF}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>